<commit_message>
minor edits to Excel comparison report
</commit_message>
<xml_diff>
--- a/comparison-analysis.xlsx
+++ b/comparison-analysis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14940" yWindow="460" windowWidth="10660" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="6380" yWindow="460" windowWidth="19220" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -6950,9 +6950,6 @@
     <t>Lav 4/5, Tro 4/5</t>
   </si>
   <si>
-    <t>Rad 5/8, Aka 5/8</t>
-  </si>
-  <si>
     <t>Note</t>
   </si>
   <si>
@@ -7071,6 +7068,9 @@
   </si>
   <si>
     <t>Tro 7/8</t>
+  </si>
+  <si>
+    <t>Rad 5/8, Aka 5/8 are neutral because of transposition</t>
   </si>
 </sst>
 </file>
@@ -7430,10 +7430,10 @@
   <dimension ref="A1:F2298"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B41" sqref="B41"/>
+      <selection pane="bottomRight" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7451,7 +7451,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>2325</v>
+        <v>2324</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>38</v>
@@ -7463,7 +7463,7 @@
         <v>39</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>2308</v>
+        <v>2307</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -7534,14 +7534,14 @@
       <c r="A7" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1" t="s">
-        <v>2307</v>
-      </c>
+      <c r="B7" s="1" t="s">
+        <v>2347</v>
+      </c>
+      <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>2309</v>
+        <v>2308</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -7549,12 +7549,12 @@
         <v>49</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>2311</v>
+        <v>2310</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
-        <v>2310</v>
+        <v>2309</v>
       </c>
       <c r="F8" s="1"/>
     </row>
@@ -7563,7 +7563,7 @@
         <v>50</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>2312</v>
+        <v>2311</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -7575,7 +7575,7 @@
         <v>51</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>2313</v>
+        <v>2312</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -7590,10 +7590,10 @@
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1" t="s">
+        <v>2313</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>2314</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>2315</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -7601,13 +7601,13 @@
         <v>53</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>2316</v>
+        <v>2315</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
-        <v>2309</v>
+        <v>2308</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -7615,12 +7615,12 @@
         <v>54</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>2318</v>
+        <v>2317</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>2317</v>
+        <v>2316</v>
       </c>
       <c r="F13" s="1"/>
     </row>
@@ -7629,7 +7629,7 @@
         <v>55</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>2319</v>
+        <v>2318</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -7641,15 +7641,15 @@
         <v>56</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>2316</v>
+        <v>2315</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
-        <v>2320</v>
+        <v>2319</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>2309</v>
+        <v>2308</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -7657,7 +7657,7 @@
         <v>57</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>2321</v>
+        <v>2320</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -7669,7 +7669,7 @@
         <v>58</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>2322</v>
+        <v>2321</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -7681,7 +7681,7 @@
         <v>59</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>2323</v>
+        <v>2322</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -7693,11 +7693,11 @@
         <v>60</v>
       </c>
       <c r="B19" s="1"/>
-      <c r="C19" s="1" t="s">
-        <v>2324</v>
-      </c>
+      <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+      <c r="E19" s="1" t="s">
+        <v>2323</v>
+      </c>
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -7705,7 +7705,7 @@
         <v>61</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>2316</v>
+        <v>2315</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -7717,13 +7717,13 @@
         <v>62</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>2326</v>
+        <v>2325</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1" t="s">
-        <v>2327</v>
+        <v>2326</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -7743,7 +7743,7 @@
         <v>64</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>2328</v>
+        <v>2327</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -7758,7 +7758,7 @@
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1" t="s">
-        <v>2329</v>
+        <v>2328</v>
       </c>
       <c r="F24" s="1"/>
     </row>
@@ -7767,7 +7767,7 @@
         <v>66</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>2330</v>
+        <v>2329</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -7779,7 +7779,7 @@
         <v>67</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>2331</v>
+        <v>2330</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -7793,7 +7793,7 @@
         <v>68</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>2332</v>
+        <v>2331</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -7805,7 +7805,7 @@
         <v>69</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>2333</v>
+        <v>2332</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -7817,10 +7817,10 @@
         <v>70</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>2333</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>2334</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>2335</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -7831,13 +7831,13 @@
         <v>71</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>2336</v>
+        <v>2335</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1" t="s">
-        <v>2309</v>
+        <v>2308</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -7845,12 +7845,12 @@
         <v>72</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>2338</v>
+        <v>2337</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1" t="s">
-        <v>2337</v>
+        <v>2336</v>
       </c>
       <c r="F31" s="1"/>
     </row>
@@ -7859,7 +7859,7 @@
         <v>73</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>2339</v>
+        <v>2338</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -7871,7 +7871,7 @@
         <v>74</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>2330</v>
+        <v>2329</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -7883,10 +7883,10 @@
         <v>75</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>2341</v>
+        <v>2340</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>2340</v>
+        <v>2339</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -7897,12 +7897,12 @@
         <v>76</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>2342</v>
+        <v>2341</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1" t="s">
-        <v>2337</v>
+        <v>2336</v>
       </c>
       <c r="F35" s="1"/>
     </row>
@@ -7911,13 +7911,13 @@
         <v>77</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>2343</v>
+        <v>2342</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1" t="s">
-        <v>2309</v>
+        <v>2308</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -7925,7 +7925,7 @@
         <v>78</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>2344</v>
+        <v>2343</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -7937,12 +7937,12 @@
         <v>79</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>2330</v>
+        <v>2329</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1" t="s">
-        <v>2345</v>
+        <v>2344</v>
       </c>
       <c r="F38" s="1"/>
     </row>
@@ -7951,7 +7951,7 @@
         <v>80</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>2346</v>
+        <v>2345</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
@@ -7963,7 +7963,7 @@
         <v>81</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>2347</v>
+        <v>2346</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>

</xml_diff>

<commit_message>
reviewed comparison through column 19; 19,23 rearranged tokens
</commit_message>
<xml_diff>
--- a/comparison-analysis.xlsx
+++ b/comparison-analysis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6380" yWindow="460" windowWidth="19220" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="9740" yWindow="460" windowWidth="15860" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2360" uniqueCount="2348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2429" uniqueCount="2403">
   <si>
     <t>Block</t>
   </si>
@@ -7071,6 +7071,171 @@
   </si>
   <si>
     <t>Rad 5/8, Aka 5/8 are neutral because of transposition</t>
+  </si>
+  <si>
+    <t>Lav 8/9</t>
+  </si>
+  <si>
+    <t>Aka 3/4</t>
+  </si>
+  <si>
+    <t>Tro 3/4</t>
+  </si>
+  <si>
+    <t>Shakh 3/4</t>
+  </si>
+  <si>
+    <t>Adjust 11/3 and 11/4</t>
+  </si>
+  <si>
+    <t>Lav 3/4, Tro 3/4</t>
+  </si>
+  <si>
+    <t>Rad 3/4, Aka 3/4, Ipa 3/4, Ost 3/4</t>
+  </si>
+  <si>
+    <t>Rad 1/2, Aka 1/2, Aka 2/3</t>
+  </si>
+  <si>
+    <t>Aka 2/3</t>
+  </si>
+  <si>
+    <t>Rad 1/2</t>
+  </si>
+  <si>
+    <t>Fix hyphens in Rad</t>
+  </si>
+  <si>
+    <t>Lav 2/3, Ipa 5/6</t>
+  </si>
+  <si>
+    <t>Rad 4/5, Tro 6/7</t>
+  </si>
+  <si>
+    <t>Aka 1/2</t>
+  </si>
+  <si>
+    <t>Lav 8/11, Tro 8/11, Bych 8/11, Shakh 8/11, Likh 8/11</t>
+  </si>
+  <si>
+    <t>Lav 5/8</t>
+  </si>
+  <si>
+    <t>Rad 9/11, Aka 9/11</t>
+  </si>
+  <si>
+    <t>Passim, 13/8 neutral, perhaps better because longer</t>
+  </si>
+  <si>
+    <t>Ipa 2/6, Ipa 3/7</t>
+  </si>
+  <si>
+    <t>Passim 1/3 neutral because of transposition</t>
+  </si>
+  <si>
+    <t>Editorial error</t>
+  </si>
+  <si>
+    <t>Improved, but shouldn't have to be; transcription error</t>
+  </si>
+  <si>
+    <t>Rad 2/3, Aka 2/3</t>
+  </si>
+  <si>
+    <t>Lav 2/3, Ipa 2/3, Bych 2/3, Shakh 2/3, Likh 2/3, Ost 2/3</t>
+  </si>
+  <si>
+    <t>Lav 5/6, Tro 5/6</t>
+  </si>
+  <si>
+    <t>Repetition and transposition</t>
+  </si>
+  <si>
+    <t>Passim, neutral because of transposition</t>
+  </si>
+  <si>
+    <t>Error in page refs, possible repetition error</t>
+  </si>
+  <si>
+    <t>Bych 7/8; passim neutral because of (possibly erroneous) repetition</t>
+  </si>
+  <si>
+    <t>Rad 7/8, Aka 7/8</t>
+  </si>
+  <si>
+    <t>&lt;lb/&gt; error in Rad</t>
+  </si>
+  <si>
+    <t>Rad 2/3 (but error in &lt;lb/&gt;)</t>
+  </si>
+  <si>
+    <t>Rad 5/6, Aka 5/6, Xle 5/6</t>
+  </si>
+  <si>
+    <t>Aka 5/6</t>
+  </si>
+  <si>
+    <t>Ipa 1/2, Ipa 2/3</t>
+  </si>
+  <si>
+    <t>Bych 5/6, Shakh 5/6, Likh 5/6, Ost 5/6,</t>
+  </si>
+  <si>
+    <t>Lav 3/4, Bych 3/4, Likh 3/4</t>
+  </si>
+  <si>
+    <t>Shakh 7/8, Ost 7/8; passim 5/7 neutral because of transposition</t>
+  </si>
+  <si>
+    <t>Lav 6/7, Bych 6/7</t>
+  </si>
+  <si>
+    <t>Lav, Aka, Ipa, Xle transposition, but could nonetheless be improved</t>
+  </si>
+  <si>
+    <t>Bych 5/6, Shakh 5/6, Likh 5/6, Ost 5/6</t>
+  </si>
+  <si>
+    <t>Numbers, transcription error, but length would help</t>
+  </si>
+  <si>
+    <t>Aka 8/9</t>
+  </si>
+  <si>
+    <t>&lt;lb/&gt; error in Aka</t>
+  </si>
+  <si>
+    <t>Passim 2/3, neutral because of word division</t>
+  </si>
+  <si>
+    <t>Word division error Ipa 2/3</t>
+  </si>
+  <si>
+    <t>Word division error Xle 3/4 Xle 8/9</t>
+  </si>
+  <si>
+    <t>Space error in number in Ipa</t>
+  </si>
+  <si>
+    <t>Passim 3/4, neutral because of space error in Ipa</t>
+  </si>
+  <si>
+    <t>Neutral, dots are erroneous</t>
+  </si>
+  <si>
+    <t>Repair dots in Rad</t>
+  </si>
+  <si>
+    <t>Passim 4/5 improved in some ways</t>
+  </si>
+  <si>
+    <t>Passim 4/5 worse in some ways</t>
+  </si>
+  <si>
+    <t>Dots in Rad are erroneous</t>
+  </si>
+  <si>
+    <t>Uh oh! Tokens are rearranged!</t>
   </si>
 </sst>
 </file>
@@ -7430,20 +7595,20 @@
   <dimension ref="A1:F2298"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C79" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F19" sqref="F19"/>
+      <selection pane="bottomRight" activeCell="C94" sqref="C94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.5" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="67.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -7721,10 +7886,10 @@
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>2326</v>
       </c>
+      <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
@@ -7974,7 +8139,9 @@
       <c r="A41" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B41" s="1"/>
+      <c r="B41" s="1" t="s">
+        <v>2348</v>
+      </c>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
@@ -7984,7 +8151,9 @@
       <c r="A42" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B42" s="1"/>
+      <c r="B42" s="1" t="s">
+        <v>2349</v>
+      </c>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
@@ -7994,7 +8163,9 @@
       <c r="A43" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B43" s="1"/>
+      <c r="B43" s="1" t="s">
+        <v>2350</v>
+      </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
@@ -8004,7 +8175,9 @@
       <c r="A44" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B44" s="1"/>
+      <c r="B44" s="1" t="s">
+        <v>2351</v>
+      </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
@@ -8018,13 +8191,17 @@
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
+      <c r="F45" s="1" t="s">
+        <v>2352</v>
+      </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B46" s="1"/>
+      <c r="B46" s="1" t="s">
+        <v>2353</v>
+      </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
@@ -8034,7 +8211,9 @@
       <c r="A47" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B47" s="1"/>
+      <c r="B47" s="1" t="s">
+        <v>2354</v>
+      </c>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
@@ -8044,7 +8223,9 @@
       <c r="A48" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B48" s="1"/>
+      <c r="B48" s="1" t="s">
+        <v>2355</v>
+      </c>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
@@ -8054,7 +8235,9 @@
       <c r="A49" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B49" s="1"/>
+      <c r="B49" s="1" t="s">
+        <v>2356</v>
+      </c>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
@@ -8064,17 +8247,23 @@
       <c r="A50" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B50" s="1"/>
+      <c r="B50" s="1" t="s">
+        <v>2357</v>
+      </c>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
+      <c r="F50" s="1" t="s">
+        <v>2358</v>
+      </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B51" s="1"/>
+      <c r="B51" s="1" t="s">
+        <v>2329</v>
+      </c>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
@@ -8084,7 +8273,9 @@
       <c r="A52" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B52" s="1"/>
+      <c r="B52" s="1" t="s">
+        <v>2359</v>
+      </c>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
@@ -8094,7 +8285,9 @@
       <c r="A53" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B53" s="1"/>
+      <c r="B53" s="1" t="s">
+        <v>2360</v>
+      </c>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
@@ -8104,7 +8297,9 @@
       <c r="A54" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B54" s="1"/>
+      <c r="B54" s="1" t="s">
+        <v>2361</v>
+      </c>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
@@ -8114,7 +8309,9 @@
       <c r="A55" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B55" s="1"/>
+      <c r="B55" s="1" t="s">
+        <v>2362</v>
+      </c>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
@@ -8124,7 +8321,9 @@
       <c r="A56" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B56" s="1"/>
+      <c r="B56" s="1" t="s">
+        <v>2363</v>
+      </c>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
@@ -8134,7 +8333,9 @@
       <c r="A57" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B57" s="1"/>
+      <c r="B57" s="1" t="s">
+        <v>2364</v>
+      </c>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
@@ -8144,7 +8345,9 @@
       <c r="A58" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B58" s="1"/>
+      <c r="B58" s="1" t="s">
+        <v>2365</v>
+      </c>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
@@ -8154,7 +8357,9 @@
       <c r="A59" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B59" s="1"/>
+      <c r="B59" s="1" t="s">
+        <v>2366</v>
+      </c>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
@@ -8164,27 +8369,37 @@
       <c r="A60" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B60" s="1"/>
+      <c r="B60" s="1" t="s">
+        <v>2367</v>
+      </c>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
-      <c r="F60" s="1"/>
+      <c r="F60" s="1" t="s">
+        <v>2308</v>
+      </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B61" s="1"/>
+      <c r="B61" s="1" t="s">
+        <v>2369</v>
+      </c>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
-      <c r="F61" s="1"/>
+      <c r="F61" s="1" t="s">
+        <v>2368</v>
+      </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B62" s="1"/>
+      <c r="B62" s="1" t="s">
+        <v>2370</v>
+      </c>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
@@ -8194,7 +8409,9 @@
       <c r="A63" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B63" s="1"/>
+      <c r="B63" s="1" t="s">
+        <v>2371</v>
+      </c>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
@@ -8204,7 +8421,9 @@
       <c r="A64" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B64" s="1"/>
+      <c r="B64" s="1" t="s">
+        <v>2372</v>
+      </c>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
@@ -8215,36 +8434,50 @@
         <v>106</v>
       </c>
       <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
+      <c r="C65" s="1" t="s">
+        <v>2373</v>
+      </c>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
-      <c r="F65" s="1"/>
+      <c r="F65" s="1" t="s">
+        <v>2373</v>
+      </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B66" s="1"/>
+      <c r="B66" s="1" t="s">
+        <v>2374</v>
+      </c>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
-      <c r="F66" s="1"/>
+      <c r="F66" s="1" t="s">
+        <v>2308</v>
+      </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B67" s="1"/>
+      <c r="B67" s="1" t="s">
+        <v>2376</v>
+      </c>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
-      <c r="F67" s="1"/>
+      <c r="F67" s="1" t="s">
+        <v>2375</v>
+      </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B68" s="1"/>
+      <c r="B68" s="1" t="s">
+        <v>2322</v>
+      </c>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
@@ -8254,7 +8487,9 @@
       <c r="A69" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B69" s="1"/>
+      <c r="B69" s="1" t="s">
+        <v>2374</v>
+      </c>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
@@ -8264,7 +8499,9 @@
       <c r="A70" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B70" s="1"/>
+      <c r="B70" s="1" t="s">
+        <v>2377</v>
+      </c>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
@@ -8274,7 +8511,9 @@
       <c r="A71" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B71" s="1"/>
+      <c r="B71" s="1" t="s">
+        <v>2374</v>
+      </c>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
@@ -8285,16 +8524,22 @@
         <v>113</v>
       </c>
       <c r="B72" s="1"/>
-      <c r="C72" s="1"/>
+      <c r="C72" s="1" t="s">
+        <v>2379</v>
+      </c>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
-      <c r="F72" s="1"/>
+      <c r="F72" s="1" t="s">
+        <v>2378</v>
+      </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B73" s="1"/>
+      <c r="B73" s="1" t="s">
+        <v>2380</v>
+      </c>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
@@ -8304,7 +8549,9 @@
       <c r="A74" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B74" s="1"/>
+      <c r="B74" s="1" t="s">
+        <v>2329</v>
+      </c>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
@@ -8314,7 +8561,9 @@
       <c r="A75" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B75" s="1"/>
+      <c r="B75" s="1" t="s">
+        <v>2381</v>
+      </c>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
@@ -8324,7 +8573,9 @@
       <c r="A76" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B76" s="1"/>
+      <c r="B76" s="1" t="s">
+        <v>2382</v>
+      </c>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
@@ -8334,7 +8585,9 @@
       <c r="A77" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B77" s="1"/>
+      <c r="B77" s="1" t="s">
+        <v>2349</v>
+      </c>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
@@ -8344,7 +8597,9 @@
       <c r="A78" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B78" s="1"/>
+      <c r="B78" s="1" t="s">
+        <v>2383</v>
+      </c>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
@@ -8354,7 +8609,9 @@
       <c r="A79" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B79" s="1"/>
+      <c r="B79" s="1" t="s">
+        <v>2384</v>
+      </c>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
@@ -8364,17 +8621,23 @@
       <c r="A80" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B80" s="1"/>
+      <c r="B80" s="1" t="s">
+        <v>2385</v>
+      </c>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
       <c r="E80" s="1"/>
-      <c r="F80" s="1"/>
+      <c r="F80" s="1" t="s">
+        <v>2308</v>
+      </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B81" s="1"/>
+      <c r="B81" s="1" t="s">
+        <v>2386</v>
+      </c>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
@@ -8385,7 +8648,9 @@
         <v>123</v>
       </c>
       <c r="B82" s="1"/>
-      <c r="C82" s="1"/>
+      <c r="C82" s="1" t="s">
+        <v>2387</v>
+      </c>
       <c r="D82" s="1"/>
       <c r="E82" s="1"/>
       <c r="F82" s="1"/>
@@ -8395,30 +8660,42 @@
         <v>124</v>
       </c>
       <c r="B83" s="1"/>
-      <c r="C83" s="1"/>
+      <c r="C83" s="1" t="s">
+        <v>2388</v>
+      </c>
       <c r="D83" s="1"/>
       <c r="E83" s="1"/>
-      <c r="F83" s="1"/>
+      <c r="F83" s="1" t="s">
+        <v>2389</v>
+      </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B84" s="1"/>
+      <c r="B84" s="1" t="s">
+        <v>2390</v>
+      </c>
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
-      <c r="F84" s="1"/>
+      <c r="F84" s="1" t="s">
+        <v>2391</v>
+      </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B85" s="1"/>
+      <c r="B85" s="1" t="s">
+        <v>2392</v>
+      </c>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
-      <c r="F85" s="1"/>
+      <c r="F85" s="1" t="s">
+        <v>2393</v>
+      </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
@@ -8428,43 +8705,59 @@
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
-      <c r="F86" s="1"/>
+      <c r="F86" s="1" t="s">
+        <v>2394</v>
+      </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B87" s="1"/>
+      <c r="B87" s="1" t="s">
+        <v>2396</v>
+      </c>
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
-      <c r="F87" s="1"/>
+      <c r="F87" s="1" t="s">
+        <v>2395</v>
+      </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B88" s="1"/>
+      <c r="B88" s="1" t="s">
+        <v>2397</v>
+      </c>
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
-      <c r="F88" s="1"/>
+      <c r="F88" s="1" t="s">
+        <v>2398</v>
+      </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B89" s="1"/>
+      <c r="B89" s="1" t="s">
+        <v>2316</v>
+      </c>
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
-      <c r="F89" s="1"/>
+      <c r="F89" s="1" t="s">
+        <v>2395</v>
+      </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B90" s="1"/>
+      <c r="B90" s="1" t="s">
+        <v>2381</v>
+      </c>
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
@@ -8474,8 +8767,12 @@
       <c r="A91" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B91" s="1"/>
-      <c r="C91" s="1"/>
+      <c r="B91" s="1" t="s">
+        <v>2399</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>2400</v>
+      </c>
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
@@ -8488,7 +8785,9 @@
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
-      <c r="F92" s="1"/>
+      <c r="F92" s="1" t="s">
+        <v>2401</v>
+      </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
@@ -8498,14 +8797,18 @@
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
       <c r="E93" s="1"/>
-      <c r="F93" s="1"/>
+      <c r="F93" s="1" t="s">
+        <v>2401</v>
+      </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>135</v>
       </c>
       <c r="B94" s="1"/>
-      <c r="C94" s="1"/>
+      <c r="C94" s="1" t="s">
+        <v>2402</v>
+      </c>
       <c r="D94" s="1"/>
       <c r="E94" s="1"/>
       <c r="F94" s="1"/>
@@ -30552,5 +30855,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>